<commit_message>
Added more test items.
</commit_message>
<xml_diff>
--- a/calc/text-angled-with-border.xlsx
+++ b/calc/text-angled-with-border.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="11">
   <si>
     <t>Field 1</t>
   </si>
@@ -37,16 +37,34 @@
   </si>
   <si>
     <t>60 degrees, right-aligned</t>
+  </si>
+  <si>
+    <t>Bordered</t>
+  </si>
+  <si>
+    <t>No borders</t>
+  </si>
+  <si>
+    <t>Vertically bordered</t>
+  </si>
+  <si>
+    <t>Bottom bordered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -80,11 +98,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
@@ -93,6 +131,35 @@
       <alignment horizontal="left" textRotation="30"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="60"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="30"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="60"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="30"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="60"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="30"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="60"/>
     </xf>
   </cellXfs>
@@ -389,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -400,66 +467,248 @@
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="32.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="32.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="27.75">
-      <c r="A5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="27.75">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="35.25">
-      <c r="A8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="35.25">
+      <c r="A9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="32.25">
+      <c r="A13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" ht="27.75">
+      <c r="A16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" ht="35.25">
+      <c r="A19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>